<commit_message>
test the d & a
</commit_message>
<xml_diff>
--- a/backend/model/main/model.xlsx
+++ b/backend/model/main/model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19739\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8316398D-FD03-43B4-AF48-A9901DA0F6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99E72103-4C50-458E-97AA-FD956D5BF106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3DEFC2DE-BB84-4643-8A7E-CDEBBFA5D37C}"/>
+    <workbookView xWindow="-4170" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3DEFC2DE-BB84-4643-8A7E-CDEBBFA5D37C}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>ProForma Financial Statement</t>
   </si>
@@ -225,12 +225,18 @@
   <si>
     <t>Total Capital Expenditures</t>
   </si>
+  <si>
+    <t>Stock:</t>
+  </si>
+  <si>
+    <t>Number Format:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="12">
+  <numFmts count="11">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0_);\(&quot;$&quot;#,##0.0\)"/>
@@ -241,8 +247,7 @@
     <numFmt numFmtId="170" formatCode="0.0\x_);&quot;NM&quot;_);0.0\x_);@_)"/>
     <numFmt numFmtId="171" formatCode="&quot;Growth&quot;"/>
     <numFmt numFmtId="172" formatCode="0.0%_);\(0.0%\);0.0%_);@_)"/>
-    <numFmt numFmtId="173" formatCode="0.0_);\(0.0\)"/>
-    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="173" formatCode="0.0%"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -652,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -830,32 +835,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="22" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="22" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1172,15 +1180,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384FE668-0B94-462B-952A-ED83A3806515}">
   <dimension ref="B1:R80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="U60" sqref="U60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="10.85546875" customWidth="1"/>
     <col min="18" max="18" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1198,10 +1205,14 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="M1" s="143" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="143"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="140" t="s">
+        <v>62</v>
+      </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="3"/>
     </row>
@@ -2347,18 +2358,18 @@
     </row>
     <row r="52" spans="2:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="97"/>
-      <c r="F52" s="131" t="s">
+      <c r="F52" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="G52" s="131"/>
-      <c r="H52" s="131"/>
-      <c r="I52" s="132" t="s">
+      <c r="G52" s="141"/>
+      <c r="H52" s="141"/>
+      <c r="I52" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="J52" s="132"/>
-      <c r="K52" s="132"/>
-      <c r="L52" s="132"/>
-      <c r="M52" s="132"/>
+      <c r="J52" s="142"/>
+      <c r="K52" s="142"/>
+      <c r="L52" s="142"/>
+      <c r="M52" s="142"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.25">
@@ -2408,7 +2419,7 @@
         <v>19</v>
       </c>
       <c r="F55" s="123">
-        <v>8000</v>
+        <v>777777.77</v>
       </c>
       <c r="G55" s="123">
         <v>9000</v>
@@ -2442,28 +2453,28 @@
       <c r="B56" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="F56" s="144"/>
-      <c r="G56" s="144">
+      <c r="F56" s="134"/>
+      <c r="G56" s="134">
         <f>(G55/F55)-1</f>
-        <v>0.125</v>
-      </c>
-      <c r="H56" s="144">
+        <v>-0.98842857131285711</v>
+      </c>
+      <c r="H56" s="134">
         <f>(H55/G55)-1</f>
         <v>0.11111111111111116</v>
       </c>
-      <c r="I56" s="146">
+      <c r="I56" s="136">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J56" s="146">
+      <c r="J56" s="136">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K56" s="146">
+      <c r="K56" s="136">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L56" s="146">
+      <c r="L56" s="136">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M56" s="146">
+      <c r="M56" s="136">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q56" s="13"/>
@@ -2517,32 +2528,32 @@
       <c r="B59" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="F59" s="127">
+      <c r="F59" s="137">
         <v>5000</v>
       </c>
-      <c r="G59" s="127">
+      <c r="G59" s="137">
         <v>6000</v>
       </c>
-      <c r="H59" s="127">
+      <c r="H59" s="137">
         <v>7000</v>
       </c>
-      <c r="I59" s="128">
+      <c r="I59" s="138">
         <f>I55*I60</f>
         <v>7489.9999999999991</v>
       </c>
-      <c r="J59" s="128">
+      <c r="J59" s="138">
         <f t="shared" ref="J59:M59" si="25">J55*J60</f>
         <v>8014.2999999999993</v>
       </c>
-      <c r="K59" s="128">
+      <c r="K59" s="138">
         <f t="shared" si="25"/>
         <v>8575.3009999999995</v>
       </c>
-      <c r="L59" s="128">
+      <c r="L59" s="138">
         <f t="shared" si="25"/>
         <v>9175.5720700000002</v>
       </c>
-      <c r="M59" s="128">
+      <c r="M59" s="138">
         <f t="shared" si="25"/>
         <v>9817.862114900001</v>
       </c>
@@ -2552,31 +2563,31 @@
       <c r="B60" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="F60" s="144">
+      <c r="F60" s="134">
         <f>F59/F55</f>
-        <v>0.625</v>
-      </c>
-      <c r="G60" s="144">
+        <v>6.4285714928571432E-3</v>
+      </c>
+      <c r="G60" s="134">
         <f>G59/G55</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="H60" s="144">
+      <c r="H60" s="134">
         <f>H59/H55</f>
         <v>0.7</v>
       </c>
-      <c r="I60" s="146">
+      <c r="I60" s="136">
         <v>0.7</v>
       </c>
-      <c r="J60" s="146">
+      <c r="J60" s="136">
         <v>0.7</v>
       </c>
-      <c r="K60" s="146">
+      <c r="K60" s="136">
         <v>0.7</v>
       </c>
-      <c r="L60" s="146">
+      <c r="L60" s="136">
         <v>0.7</v>
       </c>
-      <c r="M60" s="146">
+      <c r="M60" s="136">
         <v>0.7</v>
       </c>
       <c r="Q60" s="13"/>
@@ -2592,32 +2603,32 @@
       <c r="B62" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="F62" s="127">
+      <c r="F62" s="137">
         <v>500</v>
       </c>
-      <c r="G62" s="127">
+      <c r="G62" s="137">
         <v>600</v>
       </c>
-      <c r="H62" s="127">
+      <c r="H62" s="137">
         <v>700</v>
       </c>
-      <c r="I62" s="129">
+      <c r="I62" s="127">
         <f>AVERAGE(F62:H62)</f>
         <v>600</v>
       </c>
-      <c r="J62" s="129">
+      <c r="J62" s="127">
         <f t="shared" ref="J62:M62" si="26">AVERAGE(G62:I62)</f>
         <v>633.33333333333337</v>
       </c>
-      <c r="K62" s="129">
+      <c r="K62" s="127">
         <f t="shared" si="26"/>
         <v>644.44444444444446</v>
       </c>
-      <c r="L62" s="129">
+      <c r="L62" s="127">
         <f t="shared" si="26"/>
         <v>625.92592592592598</v>
       </c>
-      <c r="M62" s="129">
+      <c r="M62" s="127">
         <f t="shared" si="26"/>
         <v>634.56790123456801</v>
       </c>
@@ -2627,35 +2638,35 @@
       <c r="B63" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="F63" s="144">
+      <c r="F63" s="134">
         <f>F62/F55</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="G63" s="144">
+        <v>6.4285714928571437E-4</v>
+      </c>
+      <c r="G63" s="134">
         <f t="shared" ref="G63:H63" si="27">G62/G55</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H63" s="144">
+      <c r="H63" s="134">
         <f t="shared" si="27"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I63" s="145">
+      <c r="I63" s="135">
         <f>I62/I55</f>
         <v>5.6074766355140186E-2</v>
       </c>
-      <c r="J63" s="145">
+      <c r="J63" s="135">
         <f t="shared" ref="J63:M63" si="28">J62/J55</f>
         <v>5.5317786123970071E-2</v>
       </c>
-      <c r="K63" s="145">
+      <c r="K63" s="135">
         <f t="shared" si="28"/>
         <v>5.2605863177410464E-2</v>
       </c>
-      <c r="L63" s="145">
+      <c r="L63" s="135">
         <f t="shared" si="28"/>
         <v>4.7751589198530286E-2</v>
       </c>
-      <c r="M63" s="145">
+      <c r="M63" s="135">
         <f t="shared" si="28"/>
         <v>4.524381435242044E-2</v>
       </c>
@@ -2672,35 +2683,35 @@
       <c r="B65" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="F65" s="134">
+      <c r="F65" s="125">
         <f>F66+F69</f>
         <v>1000</v>
       </c>
-      <c r="G65" s="134">
+      <c r="G65" s="125">
         <f t="shared" ref="G65:H65" si="29">G66+G69</f>
         <v>1200</v>
       </c>
-      <c r="H65" s="134">
+      <c r="H65" s="125">
         <f t="shared" si="29"/>
         <v>1400</v>
       </c>
-      <c r="I65" s="135">
+      <c r="I65" s="126">
         <f>I66+I69</f>
         <v>1498.0000000000002</v>
       </c>
-      <c r="J65" s="135">
+      <c r="J65" s="126">
         <f t="shared" ref="J65:M65" si="30">J66+J69</f>
         <v>1602.8600000000001</v>
       </c>
-      <c r="K65" s="135">
+      <c r="K65" s="126">
         <f t="shared" si="30"/>
         <v>1715.0602000000001</v>
       </c>
-      <c r="L65" s="135">
+      <c r="L65" s="126">
         <f t="shared" si="30"/>
         <v>1835.1144140000001</v>
       </c>
-      <c r="M65" s="135">
+      <c r="M65" s="126">
         <f t="shared" si="30"/>
         <v>1963.5724229800005</v>
       </c>
@@ -2710,32 +2721,32 @@
       <c r="B66" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="F66" s="127">
+      <c r="F66" s="137">
         <v>500</v>
       </c>
-      <c r="G66" s="127">
+      <c r="G66" s="137">
         <v>600</v>
       </c>
-      <c r="H66" s="127">
+      <c r="H66" s="137">
         <v>700</v>
       </c>
-      <c r="I66" s="128">
+      <c r="I66" s="138">
         <f>I67*I55</f>
         <v>749.00000000000011</v>
       </c>
-      <c r="J66" s="128">
+      <c r="J66" s="138">
         <f t="shared" ref="J66:M66" si="31">J67*J55</f>
         <v>801.43000000000006</v>
       </c>
-      <c r="K66" s="128">
+      <c r="K66" s="138">
         <f t="shared" si="31"/>
         <v>857.53010000000006</v>
       </c>
-      <c r="L66" s="128">
+      <c r="L66" s="138">
         <f t="shared" si="31"/>
         <v>917.55720700000006</v>
       </c>
-      <c r="M66" s="128">
+      <c r="M66" s="138">
         <f t="shared" si="31"/>
         <v>981.78621149000026</v>
       </c>
@@ -2745,31 +2756,31 @@
       <c r="B67" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="F67" s="140">
+      <c r="F67" s="130">
         <f>F66/F55</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="G67" s="140">
+        <v>6.4285714928571437E-4</v>
+      </c>
+      <c r="G67" s="130">
         <f t="shared" ref="G67:H67" si="32">G66/G55</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H67" s="140">
+      <c r="H67" s="130">
         <f t="shared" si="32"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I67" s="143">
+      <c r="I67" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J67" s="143">
+      <c r="J67" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K67" s="143">
+      <c r="K67" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L67" s="143">
+      <c r="L67" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M67" s="143">
+      <c r="M67" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q67" s="13"/>
@@ -2785,32 +2796,32 @@
       <c r="B69" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="F69" s="127">
+      <c r="F69" s="137">
         <v>500</v>
       </c>
-      <c r="G69" s="127">
+      <c r="G69" s="137">
         <v>600</v>
       </c>
-      <c r="H69" s="127">
+      <c r="H69" s="137">
         <v>700</v>
       </c>
-      <c r="I69" s="128">
+      <c r="I69" s="138">
         <f>I70*I55</f>
         <v>749.00000000000011</v>
       </c>
-      <c r="J69" s="128">
+      <c r="J69" s="138">
         <f t="shared" ref="J69:M69" si="33">J70*J55</f>
         <v>801.43000000000006</v>
       </c>
-      <c r="K69" s="128">
+      <c r="K69" s="138">
         <f t="shared" si="33"/>
         <v>857.53010000000006</v>
       </c>
-      <c r="L69" s="128">
+      <c r="L69" s="138">
         <f t="shared" si="33"/>
         <v>917.55720700000006</v>
       </c>
-      <c r="M69" s="128">
+      <c r="M69" s="138">
         <f t="shared" si="33"/>
         <v>981.78621149000026</v>
       </c>
@@ -2820,31 +2831,31 @@
       <c r="B70" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="F70" s="140">
+      <c r="F70" s="130">
         <f>F69/F55</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="G70" s="140">
+        <v>6.4285714928571437E-4</v>
+      </c>
+      <c r="G70" s="130">
         <f t="shared" ref="G70:H70" si="34">G69/G55</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H70" s="140">
+      <c r="H70" s="130">
         <f t="shared" si="34"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I70" s="143">
+      <c r="I70" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J70" s="143">
+      <c r="J70" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K70" s="143">
+      <c r="K70" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L70" s="143">
+      <c r="L70" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M70" s="143">
+      <c r="M70" s="133">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q70" s="13"/>
@@ -2860,35 +2871,35 @@
       <c r="B72" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="F72" s="136">
+      <c r="F72" s="125">
         <f>F55-SUM(F58,F65)</f>
-        <v>1500</v>
-      </c>
-      <c r="G72" s="136">
+        <v>771277.77</v>
+      </c>
+      <c r="G72" s="125">
         <f t="shared" ref="G72:M72" si="35">G55-SUM(G58,G65)</f>
         <v>1200</v>
       </c>
-      <c r="H72" s="136">
+      <c r="H72" s="125">
         <f t="shared" si="35"/>
         <v>900</v>
       </c>
-      <c r="I72" s="137">
+      <c r="I72" s="139">
         <f t="shared" si="35"/>
         <v>1112</v>
       </c>
-      <c r="J72" s="137">
+      <c r="J72" s="139">
         <f t="shared" si="35"/>
         <v>1198.5066666666662</v>
       </c>
-      <c r="K72" s="137">
+      <c r="K72" s="139">
         <f t="shared" si="35"/>
         <v>1315.6243555555557</v>
       </c>
-      <c r="L72" s="137">
+      <c r="L72" s="139">
         <f t="shared" si="35"/>
         <v>1471.3476900740752</v>
       </c>
-      <c r="M72" s="137">
+      <c r="M72" s="139">
         <f t="shared" si="35"/>
         <v>1609.514867885433</v>
       </c>
@@ -2898,35 +2909,35 @@
       <c r="B73" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="F73" s="140">
+      <c r="F73" s="130">
         <f>F72/F55</f>
-        <v>0.1875</v>
-      </c>
-      <c r="G73" s="140">
+        <v>0.99164285705928568</v>
+      </c>
+      <c r="G73" s="130">
         <f t="shared" ref="G73:M73" si="36">G72/G55</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="H73" s="140">
+      <c r="H73" s="130">
         <f t="shared" si="36"/>
         <v>0.09</v>
       </c>
-      <c r="I73" s="141">
+      <c r="I73" s="131">
         <f t="shared" si="36"/>
         <v>0.10392523364485981</v>
       </c>
-      <c r="J73" s="141">
+      <c r="J73" s="131">
         <f t="shared" si="36"/>
         <v>0.10468221387602988</v>
       </c>
-      <c r="K73" s="141">
+      <c r="K73" s="131">
         <f t="shared" si="36"/>
         <v>0.10739413682258954</v>
       </c>
-      <c r="L73" s="141">
+      <c r="L73" s="131">
         <f t="shared" si="36"/>
         <v>0.1122484108014698</v>
       </c>
-      <c r="M73" s="141">
+      <c r="M73" s="131">
         <f t="shared" si="36"/>
         <v>0.11475618564757961</v>
       </c>
@@ -2945,7 +2956,7 @@
       </c>
       <c r="F75" s="125">
         <f>F72+F62</f>
-        <v>2000</v>
+        <v>771777.77</v>
       </c>
       <c r="G75" s="125">
         <f t="shared" ref="G75:M75" si="37">G72+G62</f>
@@ -2955,23 +2966,23 @@
         <f t="shared" si="37"/>
         <v>1600</v>
       </c>
-      <c r="I75" s="133">
+      <c r="I75" s="139">
         <f t="shared" si="37"/>
         <v>1712</v>
       </c>
-      <c r="J75" s="133">
+      <c r="J75" s="139">
         <f t="shared" si="37"/>
         <v>1831.8399999999997</v>
       </c>
-      <c r="K75" s="133">
+      <c r="K75" s="139">
         <f t="shared" si="37"/>
         <v>1960.0688</v>
       </c>
-      <c r="L75" s="133">
+      <c r="L75" s="139">
         <f t="shared" si="37"/>
         <v>2097.2736160000013</v>
       </c>
-      <c r="M75" s="133">
+      <c r="M75" s="139">
         <f t="shared" si="37"/>
         <v>2244.0827691200011</v>
       </c>
@@ -2981,35 +2992,35 @@
       <c r="B76" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="F76" s="140">
+      <c r="F76" s="130">
         <f>F75/F55</f>
-        <v>0.25</v>
-      </c>
-      <c r="G76" s="140">
+        <v>0.99228571420857148</v>
+      </c>
+      <c r="G76" s="130">
         <f t="shared" ref="G76:H76" si="38">G75/G55</f>
         <v>0.2</v>
       </c>
-      <c r="H76" s="140">
+      <c r="H76" s="130">
         <f t="shared" si="38"/>
         <v>0.16</v>
       </c>
-      <c r="I76" s="142">
+      <c r="I76" s="132">
         <f>I75/I55</f>
         <v>0.16</v>
       </c>
-      <c r="J76" s="142">
+      <c r="J76" s="132">
         <f t="shared" ref="J76:M76" si="39">J75/J55</f>
         <v>0.15999999999999998</v>
       </c>
-      <c r="K76" s="142">
+      <c r="K76" s="132">
         <f t="shared" si="39"/>
         <v>0.16</v>
       </c>
-      <c r="L76" s="142">
+      <c r="L76" s="132">
         <f t="shared" si="39"/>
         <v>0.16000000000000009</v>
       </c>
-      <c r="M76" s="142">
+      <c r="M76" s="132">
         <f t="shared" si="39"/>
         <v>0.16000000000000006</v>
       </c>
@@ -3019,32 +3030,32 @@
       <c r="B77" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="F77" s="140"/>
-      <c r="G77" s="140">
+      <c r="F77" s="130"/>
+      <c r="G77" s="130">
         <f>G75/F75-1</f>
-        <v>-9.9999999999999978E-2</v>
-      </c>
-      <c r="H77" s="140">
+        <v>-0.99766772240667156</v>
+      </c>
+      <c r="H77" s="130">
         <f>H75/G75-1</f>
         <v>-0.11111111111111116</v>
       </c>
-      <c r="I77" s="142">
+      <c r="I77" s="132">
         <f>I75/H75-1</f>
         <v>7.0000000000000062E-2</v>
       </c>
-      <c r="J77" s="142">
+      <c r="J77" s="132">
         <f t="shared" ref="J77:M77" si="40">J75/I75-1</f>
         <v>6.999999999999984E-2</v>
       </c>
-      <c r="K77" s="142">
+      <c r="K77" s="132">
         <f t="shared" si="40"/>
         <v>7.0000000000000284E-2</v>
       </c>
-      <c r="L77" s="142">
+      <c r="L77" s="132">
         <f t="shared" si="40"/>
         <v>7.0000000000000728E-2</v>
       </c>
-      <c r="M77" s="142">
+      <c r="M77" s="132">
         <f t="shared" si="40"/>
         <v>6.999999999999984E-2</v>
       </c>
@@ -3061,28 +3072,28 @@
       <c r="B79" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="F79" s="127">
+      <c r="F79" s="144">
         <v>200</v>
       </c>
-      <c r="G79" s="127">
+      <c r="G79" s="144">
         <v>300</v>
       </c>
-      <c r="H79" s="127">
+      <c r="H79" s="144">
         <v>300</v>
       </c>
-      <c r="I79" s="130">
+      <c r="I79" s="145">
         <v>300</v>
       </c>
-      <c r="J79" s="130">
+      <c r="J79" s="145">
         <v>300</v>
       </c>
-      <c r="K79" s="130">
+      <c r="K79" s="145">
         <v>300</v>
       </c>
-      <c r="L79" s="130">
+      <c r="L79" s="145">
         <v>300</v>
       </c>
-      <c r="M79" s="130">
+      <c r="M79" s="145">
         <v>300</v>
       </c>
       <c r="Q79" s="13"/>
@@ -3094,35 +3105,35 @@
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
-      <c r="F80" s="138">
+      <c r="F80" s="128">
         <f>F79/F55</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G80" s="138">
+        <v>2.5714285971428574E-4</v>
+      </c>
+      <c r="G80" s="128">
         <f t="shared" ref="G80:H80" si="41">G79/G55</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="H80" s="138">
+      <c r="H80" s="128">
         <f t="shared" si="41"/>
         <v>0.03</v>
       </c>
-      <c r="I80" s="139">
+      <c r="I80" s="129">
         <f>I79/I55</f>
         <v>2.8037383177570093E-2</v>
       </c>
-      <c r="J80" s="139">
+      <c r="J80" s="129">
         <f t="shared" ref="J80:M80" si="42">J79/J55</f>
         <v>2.6203161848196349E-2</v>
       </c>
-      <c r="K80" s="139">
+      <c r="K80" s="129">
         <f t="shared" si="42"/>
         <v>2.4488936306725561E-2</v>
       </c>
-      <c r="L80" s="139">
+      <c r="L80" s="129">
         <f t="shared" si="42"/>
         <v>2.2886856361425758E-2</v>
       </c>
-      <c r="M80" s="139">
+      <c r="M80" s="129">
         <f t="shared" si="42"/>
         <v>2.1389585384510051E-2</v>
       </c>
@@ -3132,9 +3143,10 @@
       <c r="Q80" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="F52:H52"/>
     <mergeCell ref="I52:M52"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>